<commit_message>
Lowered min velocity level to 36km/h in FCW status computing.
</commit_message>
<xml_diff>
--- a/Road_Data.xlsx
+++ b/Road_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamg\OneDrive\Počítač\DP_Implementacia_Final\Matlab\Work_version\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamg\OneDrive\Počítač\DP_Implementacia_Final\Matlab\DP3\DP3_FCW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E54F8CA-B88B-4D2C-85CE-65AADFC81ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D31B14-8A08-4130-8B31-ABA3D35A25A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28425" yWindow="540" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6060" yWindow="1470" windowWidth="20295" windowHeight="13875" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioTest" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Scenario2" sheetId="5" r:id="rId3"/>
     <sheet name="Scenario3" sheetId="3" r:id="rId4"/>
     <sheet name="Scenario4" sheetId="6" r:id="rId5"/>
+    <sheet name="Scenario5" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="12">
   <si>
     <t>Time</t>
   </si>
@@ -67,6 +68,12 @@
   </si>
   <si>
     <t>Acceleration</t>
+  </si>
+  <si>
+    <t>DecelerationLead</t>
+  </si>
+  <si>
+    <t>Gear</t>
   </si>
 </sst>
 </file>
@@ -559,7 +566,7 @@
   <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I54"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2140,7 +2147,7 @@
   <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3721,7 +3728,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4005,7 +4012,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E421FB8-57D5-4889-88A6-C82D7D1032D6}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
@@ -4284,4 +4291,1913 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1D5B72A-21DA-4909-945D-87FCE1226833}">
+  <dimension ref="A1:K54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>21.94134</v>
+      </c>
+      <c r="C2">
+        <v>48.989939999999997</v>
+      </c>
+      <c r="D2">
+        <v>10.925040450571499</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1E-10</v>
+      </c>
+      <c r="F2">
+        <v>-2.0327558290333601</v>
+      </c>
+      <c r="G2">
+        <v>17.320030699483201</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>21.941210000000002</v>
+      </c>
+      <c r="C3">
+        <v>48.989179999999998</v>
+      </c>
+      <c r="D3">
+        <v>14.133507802330801</v>
+      </c>
+      <c r="E3">
+        <v>-2.1628328061320898E-2</v>
+      </c>
+      <c r="F3">
+        <v>-0.943545904088818</v>
+      </c>
+      <c r="G3">
+        <v>89.247489405984894</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>-0.94499201340343897</v>
+      </c>
+      <c r="K3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>21.94117</v>
+      </c>
+      <c r="C4">
+        <v>48.988869999999999</v>
+      </c>
+      <c r="D4">
+        <v>10.622369063027101</v>
+      </c>
+      <c r="E4">
+        <v>-0.11368961847077</v>
+      </c>
+      <c r="F4">
+        <v>0.90247780987982595</v>
+      </c>
+      <c r="G4">
+        <v>114.54209702669</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0.91224139229994805</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>21.94115</v>
+      </c>
+      <c r="C5">
+        <v>48.988379999999999</v>
+      </c>
+      <c r="D5">
+        <v>14.792673114446099</v>
+      </c>
+      <c r="E5">
+        <v>-0.30590293607049301</v>
+      </c>
+      <c r="F5">
+        <v>-1.5456229865917399</v>
+      </c>
+      <c r="G5">
+        <v>148.804511735929</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>-1.57826039326243</v>
+      </c>
+      <c r="K5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>21.941109999999998</v>
+      </c>
+      <c r="C6">
+        <v>48.986370000000001</v>
+      </c>
+      <c r="D6">
+        <v>11.429654360072201</v>
+      </c>
+      <c r="E6">
+        <v>4.7971126412152901E-3</v>
+      </c>
+      <c r="F6">
+        <v>1.21831190208328</v>
+      </c>
+      <c r="G6">
+        <v>145.512802864794</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>1.2178007818568</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>21.94107</v>
+      </c>
+      <c r="C7">
+        <v>48.984630000000003</v>
+      </c>
+      <c r="D7">
+        <v>14.558102400024101</v>
+      </c>
+      <c r="E7">
+        <v>-0.12652309854476401</v>
+      </c>
+      <c r="F7">
+        <v>-2.38204119025318</v>
+      </c>
+      <c r="G7">
+        <v>146.62767695613101</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>-2.4029247835145999</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>21.940899999999999</v>
+      </c>
+      <c r="C8">
+        <v>48.977049999999998</v>
+      </c>
+      <c r="D8">
+        <v>14.2590431699162</v>
+      </c>
+      <c r="E8">
+        <v>1.10908132428938E-2</v>
+      </c>
+      <c r="F8">
+        <v>2.0512942979127899</v>
+      </c>
+      <c r="G8">
+        <v>141.93473053875499</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>2.04970002262489</v>
+      </c>
+      <c r="K8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>21.94089</v>
+      </c>
+      <c r="C9">
+        <v>48.976469999999999</v>
+      </c>
+      <c r="D9">
+        <v>10.472803493232499</v>
+      </c>
+      <c r="E9">
+        <v>0.50236151044288002</v>
+      </c>
+      <c r="F9">
+        <v>2.1210753203204198</v>
+      </c>
+      <c r="G9">
+        <v>140.99084704749799</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>2.02398825134948</v>
+      </c>
+      <c r="K9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>21.94089</v>
+      </c>
+      <c r="C10">
+        <v>48.976379999999999</v>
+      </c>
+      <c r="D10">
+        <v>10.9408563926377</v>
+      </c>
+      <c r="E10">
+        <v>9.5225803239573997E-2</v>
+      </c>
+      <c r="F10">
+        <v>-1.96276922684734</v>
+      </c>
+      <c r="G10">
+        <v>145.63410800681899</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>-1.9458333004123001</v>
+      </c>
+      <c r="K10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>21.94089</v>
+      </c>
+      <c r="C11">
+        <v>48.974730000000001</v>
+      </c>
+      <c r="D11">
+        <v>14.2693099576928</v>
+      </c>
+      <c r="E11">
+        <v>-5.1988264133124899E-2</v>
+      </c>
+      <c r="F11">
+        <v>-1.2982385323335699</v>
+      </c>
+      <c r="G11">
+        <v>145.81109258127501</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>-1.30298578144149</v>
+      </c>
+      <c r="K11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>21.940909999999999</v>
+      </c>
+      <c r="C12">
+        <v>48.974510000000002</v>
+      </c>
+      <c r="D12">
+        <v>13.8345471943188</v>
+      </c>
+      <c r="E12">
+        <v>-0.229428549814086</v>
+      </c>
+      <c r="F12">
+        <v>0.95900201083709602</v>
+      </c>
+      <c r="G12">
+        <v>146.851254438925</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0.97517404478727499</v>
+      </c>
+      <c r="K12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>21.940950000000001</v>
+      </c>
+      <c r="C13">
+        <v>48.97437</v>
+      </c>
+      <c r="D13">
+        <v>13.4388450925886</v>
+      </c>
+      <c r="E13">
+        <v>0.227910346175343</v>
+      </c>
+      <c r="F13">
+        <v>2.2060769884094702</v>
+      </c>
+      <c r="G13">
+        <v>142.526057580535</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>2.16928787834083</v>
+      </c>
+      <c r="K13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>21.941030000000001</v>
+      </c>
+      <c r="C14">
+        <v>48.974179999999997</v>
+      </c>
+      <c r="D14">
+        <v>11.062503956796499</v>
+      </c>
+      <c r="E14">
+        <v>0.72360769528245295</v>
+      </c>
+      <c r="F14">
+        <v>0.74026364961218305</v>
+      </c>
+      <c r="G14">
+        <v>140.629363880352</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0.69481520238805095</v>
+      </c>
+      <c r="K14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>21.941109999999998</v>
+      </c>
+      <c r="C15">
+        <v>48.974049999999998</v>
+      </c>
+      <c r="D15">
+        <v>10.9810129362748</v>
+      </c>
+      <c r="E15">
+        <v>0.55559907004352405</v>
+      </c>
+      <c r="F15">
+        <v>1.52672233962526</v>
+      </c>
+      <c r="G15">
+        <v>147.71359087675299</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>1.4531959428247201</v>
+      </c>
+      <c r="K15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>21.941269999999999</v>
+      </c>
+      <c r="C16">
+        <v>48.973849999999999</v>
+      </c>
+      <c r="D16">
+        <v>15.428378541874499</v>
+      </c>
+      <c r="E16">
+        <v>0.64654339037783004</v>
+      </c>
+      <c r="F16">
+        <v>-2.11087801044645</v>
+      </c>
+      <c r="G16">
+        <v>147.70240552708</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>-2.0259771797425801</v>
+      </c>
+      <c r="K16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>21.942519999999998</v>
+      </c>
+      <c r="C17">
+        <v>48.972439999999999</v>
+      </c>
+      <c r="D17">
+        <v>12.632800010436201</v>
+      </c>
+      <c r="E17">
+        <v>0.812953298497753</v>
+      </c>
+      <c r="F17">
+        <v>1.9921011368737001</v>
+      </c>
+      <c r="G17">
+        <v>146.39514605631601</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>1.87165528657786</v>
+      </c>
+      <c r="K17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>21.943670000000001</v>
+      </c>
+      <c r="C18">
+        <v>48.971119999999999</v>
+      </c>
+      <c r="D18">
+        <v>10.6477842237242</v>
+      </c>
+      <c r="E18">
+        <v>0.46686102929012102</v>
+      </c>
+      <c r="F18">
+        <v>1.67824674996476</v>
+      </c>
+      <c r="G18">
+        <v>148.16697363462399</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>1.60775345150534</v>
+      </c>
+      <c r="K18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>21.945489999999999</v>
+      </c>
+      <c r="C19">
+        <v>48.969009999999997</v>
+      </c>
+      <c r="D19">
+        <v>16.2611815085777</v>
+      </c>
+      <c r="E19">
+        <v>0.50203556082636103</v>
+      </c>
+      <c r="F19">
+        <v>-3.5377294834537101</v>
+      </c>
+      <c r="G19">
+        <v>143.89771731413001</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>-3.43177929513817</v>
+      </c>
+      <c r="K19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>21.94595</v>
+      </c>
+      <c r="C20">
+        <v>48.96848</v>
+      </c>
+      <c r="D20">
+        <v>10.704414052963701</v>
+      </c>
+      <c r="E20">
+        <v>3.5559888140374397E-2</v>
+      </c>
+      <c r="F20">
+        <v>0.89847192185931501</v>
+      </c>
+      <c r="G20">
+        <v>146.097751121572</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0.89549709517781695</v>
+      </c>
+      <c r="K20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>21.94631</v>
+      </c>
+      <c r="C21">
+        <v>48.967979999999997</v>
+      </c>
+      <c r="D21">
+        <v>17.299789414949899</v>
+      </c>
+      <c r="E21">
+        <v>-0.29848249552835499</v>
+      </c>
+      <c r="F21">
+        <v>-2.7815815291479602</v>
+      </c>
+      <c r="G21">
+        <v>149.752807116908</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>-2.83041620993284</v>
+      </c>
+      <c r="K21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>21.946580000000001</v>
+      </c>
+      <c r="C22">
+        <v>48.967590000000001</v>
+      </c>
+      <c r="D22">
+        <v>13.7024927800274</v>
+      </c>
+      <c r="E22">
+        <v>0.12571434404798201</v>
+      </c>
+      <c r="F22">
+        <v>2.2566074988864702</v>
+      </c>
+      <c r="G22">
+        <v>144.86193652987399</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>2.2360923352827702</v>
+      </c>
+      <c r="K22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>21.946739999999998</v>
+      </c>
+      <c r="C23">
+        <v>48.96725</v>
+      </c>
+      <c r="D23">
+        <v>14.1301843023909</v>
+      </c>
+      <c r="E23">
+        <v>-0.302751239476302</v>
+      </c>
+      <c r="F23">
+        <v>-3.5591516692695699</v>
+      </c>
+      <c r="G23">
+        <v>147.062615757147</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>-3.6370791901950099</v>
+      </c>
+      <c r="K23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>21.946819999999999</v>
+      </c>
+      <c r="C24">
+        <v>48.96698</v>
+      </c>
+      <c r="D24">
+        <v>17.462778804568501</v>
+      </c>
+      <c r="E24">
+        <v>-0.214580562494847</v>
+      </c>
+      <c r="F24">
+        <v>-0.80488873036401398</v>
+      </c>
+      <c r="G24">
+        <v>142.90098586242601</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>-0.81490215171291602</v>
+      </c>
+      <c r="K24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>21.946860000000001</v>
+      </c>
+      <c r="C25">
+        <v>48.966760000000001</v>
+      </c>
+      <c r="D25">
+        <v>17.399182736758899</v>
+      </c>
+      <c r="E25">
+        <v>8.1580971242552397E-2</v>
+      </c>
+      <c r="F25">
+        <v>1.3160152705169099</v>
+      </c>
+      <c r="G25">
+        <v>138.74830838567399</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>1.3098735592202999</v>
+      </c>
+      <c r="K25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>21.946809999999999</v>
+      </c>
+      <c r="C26">
+        <v>48.96604</v>
+      </c>
+      <c r="D26">
+        <v>16.4563530935663</v>
+      </c>
+      <c r="E26">
+        <v>-0.28305798252082398</v>
+      </c>
+      <c r="F26">
+        <v>0.41760905909432999</v>
+      </c>
+      <c r="G26">
+        <v>140.589712685465</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0.424917871364066</v>
+      </c>
+      <c r="K26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>21.946619999999999</v>
+      </c>
+      <c r="C27">
+        <v>48.964739999999999</v>
+      </c>
+      <c r="D27">
+        <v>15.038555169561199</v>
+      </c>
+      <c r="E27">
+        <v>0.18450077398057599</v>
+      </c>
+      <c r="F27">
+        <v>1.19692673196905</v>
+      </c>
+      <c r="G27">
+        <v>136.72732486669699</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>1.18242018944137</v>
+      </c>
+      <c r="K27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>21.9466</v>
+      </c>
+      <c r="C28">
+        <v>48.964590000000001</v>
+      </c>
+      <c r="D28">
+        <v>15.2445061157468</v>
+      </c>
+      <c r="E28">
+        <v>1.6846997037116299E-2</v>
+      </c>
+      <c r="F28">
+        <v>-3.985039286563</v>
+      </c>
+      <c r="G28">
+        <v>141.91064305784201</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>-3.98064020447916</v>
+      </c>
+      <c r="K28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>21.946560000000002</v>
+      </c>
+      <c r="C29">
+        <v>48.964329999999997</v>
+      </c>
+      <c r="D29">
+        <v>16.451246549422098</v>
+      </c>
+      <c r="E29">
+        <v>-0.41720249500154699</v>
+      </c>
+      <c r="F29">
+        <v>-0.29568531282549998</v>
+      </c>
+      <c r="G29">
+        <v>148.19283049742899</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>-0.30337898323250501</v>
+      </c>
+      <c r="K29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>21.946470000000001</v>
+      </c>
+      <c r="C30">
+        <v>48.963729999999998</v>
+      </c>
+      <c r="D30">
+        <v>10.360336317112401</v>
+      </c>
+      <c r="E30">
+        <v>-0.43596523420998901</v>
+      </c>
+      <c r="F30">
+        <v>0.57394262124276896</v>
+      </c>
+      <c r="G30">
+        <v>148.81710015683799</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0.59915520420676904</v>
+      </c>
+      <c r="K30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>21.946259999999999</v>
+      </c>
+      <c r="C31">
+        <v>48.962330000000001</v>
+      </c>
+      <c r="D31">
+        <v>13.5450802049931</v>
+      </c>
+      <c r="E31">
+        <v>-0.26090753838300701</v>
+      </c>
+      <c r="F31">
+        <v>-3.5449762305041799</v>
+      </c>
+      <c r="G31">
+        <v>147.02590489018601</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>-3.6146012681440398</v>
+      </c>
+      <c r="K31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>21.945969999999999</v>
+      </c>
+      <c r="C32">
+        <v>48.960360000000001</v>
+      </c>
+      <c r="D32">
+        <v>15.5528348539255</v>
+      </c>
+      <c r="E32">
+        <v>-0.43994419099119902</v>
+      </c>
+      <c r="F32">
+        <v>-1.09065585995334</v>
+      </c>
+      <c r="G32">
+        <v>147.799605458895</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>-1.12240542531835</v>
+      </c>
+      <c r="K32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>21.945489999999999</v>
+      </c>
+      <c r="C33">
+        <v>48.957129999999999</v>
+      </c>
+      <c r="D33">
+        <v>14.69984175015</v>
+      </c>
+      <c r="E33">
+        <v>-0.158834173491023</v>
+      </c>
+      <c r="F33">
+        <v>1.57280097998526</v>
+      </c>
+      <c r="G33">
+        <v>143.622953649804</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>1.5899809822928599</v>
+      </c>
+      <c r="K33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>21.9452</v>
+      </c>
+      <c r="C34">
+        <v>48.955080000000002</v>
+      </c>
+      <c r="D34">
+        <v>10.5352997437236</v>
+      </c>
+      <c r="E34">
+        <v>-0.47607883312496901</v>
+      </c>
+      <c r="F34">
+        <v>1.6314897984404699</v>
+      </c>
+      <c r="G34">
+        <v>146.648353533961</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>1.7087043030626401</v>
+      </c>
+      <c r="K34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>21.9451</v>
+      </c>
+      <c r="C35">
+        <v>48.95438</v>
+      </c>
+      <c r="D35">
+        <v>14.8499397062553</v>
+      </c>
+      <c r="E35">
+        <v>-0.93898180535724796</v>
+      </c>
+      <c r="F35">
+        <v>-3.1767767402181799</v>
+      </c>
+      <c r="G35">
+        <v>148.91782059370499</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>-3.39120737684273</v>
+      </c>
+      <c r="K35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>21.944870000000002</v>
+      </c>
+      <c r="C36">
+        <v>48.9527</v>
+      </c>
+      <c r="D36">
+        <v>15.6293688097723</v>
+      </c>
+      <c r="E36">
+        <v>-1.37673137580548</v>
+      </c>
+      <c r="F36">
+        <v>-3.4594525091611499</v>
+      </c>
+      <c r="G36">
+        <v>149.54875423362299</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>-3.7936178055518801</v>
+      </c>
+      <c r="K36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>21.94483</v>
+      </c>
+      <c r="C37">
+        <v>48.95232</v>
+      </c>
+      <c r="D37">
+        <v>11.689402491913899</v>
+      </c>
+      <c r="E37">
+        <v>-0.89441309001556701</v>
+      </c>
+      <c r="F37">
+        <v>0.79641668042237301</v>
+      </c>
+      <c r="G37">
+        <v>146.11593720837499</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>0.86240335975632898</v>
+      </c>
+      <c r="K37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>21.944780000000002</v>
+      </c>
+      <c r="C38">
+        <v>48.951970000000003</v>
+      </c>
+      <c r="D38">
+        <v>14.143350531823501</v>
+      </c>
+      <c r="E38">
+        <v>-1.30249830054184</v>
+      </c>
+      <c r="F38">
+        <v>-1.95143984924201</v>
+      </c>
+      <c r="G38">
+        <v>147.44617881890699</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>-2.14938209181804</v>
+      </c>
+      <c r="K38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>21.94455</v>
+      </c>
+      <c r="C39">
+        <v>48.949820000000003</v>
+      </c>
+      <c r="D39">
+        <v>10.786374610063</v>
+      </c>
+      <c r="E39">
+        <v>-1.1351293566888301</v>
+      </c>
+      <c r="F39">
+        <v>1.68888707078405</v>
+      </c>
+      <c r="G39">
+        <v>147.39915721801799</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>1.88752519921716</v>
+      </c>
+      <c r="K39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>21.944479999999999</v>
+      </c>
+      <c r="C40">
+        <v>48.949080000000002</v>
+      </c>
+      <c r="D40">
+        <v>15.118973130396601</v>
+      </c>
+      <c r="E40">
+        <v>-1.08305340163435</v>
+      </c>
+      <c r="F40">
+        <v>-2.2890856827008101</v>
+      </c>
+      <c r="G40">
+        <v>142.80989636832399</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>-2.4657183568106</v>
+      </c>
+      <c r="K40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>21.944420000000001</v>
+      </c>
+      <c r="C41">
+        <v>48.94847</v>
+      </c>
+      <c r="D41">
+        <v>14.308694759630299</v>
+      </c>
+      <c r="E41">
+        <v>-0.93211153465331698</v>
+      </c>
+      <c r="F41">
+        <v>0.90878497801253</v>
+      </c>
+      <c r="G41">
+        <v>137.943419279029</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>0.97211123601714899</v>
+      </c>
+      <c r="K41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>21.94426</v>
+      </c>
+      <c r="C42">
+        <v>48.947279999999999</v>
+      </c>
+      <c r="D42">
+        <v>16.7445960153538</v>
+      </c>
+      <c r="E42">
+        <v>-0.64435958876743005</v>
+      </c>
+      <c r="F42">
+        <v>-1.1501413136774501</v>
+      </c>
+      <c r="G42">
+        <v>135.47495874618701</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>-1.1961719783378699</v>
+      </c>
+      <c r="K42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>21.944140000000001</v>
+      </c>
+      <c r="C43">
+        <v>48.946829999999999</v>
+      </c>
+      <c r="D43">
+        <v>14.9070934356035</v>
+      </c>
+      <c r="E43">
+        <v>-1.10014755641113</v>
+      </c>
+      <c r="F43">
+        <v>1.5434848898515801</v>
+      </c>
+      <c r="G43">
+        <v>144.87903028848399</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>1.6664708959376</v>
+      </c>
+      <c r="K43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>21.943999999999999</v>
+      </c>
+      <c r="C44">
+        <v>48.946510000000004</v>
+      </c>
+      <c r="D44">
+        <v>15.0353104922266</v>
+      </c>
+      <c r="E44">
+        <v>-0.84373129438190098</v>
+      </c>
+      <c r="F44">
+        <v>-3.1506785693711801</v>
+      </c>
+      <c r="G44">
+        <v>142.32836526881701</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>-3.33799571501488</v>
+      </c>
+      <c r="K44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>21.943760000000001</v>
+      </c>
+      <c r="C45">
+        <v>48.946069999999999</v>
+      </c>
+      <c r="D45">
+        <v>13.638414421540601</v>
+      </c>
+      <c r="E45">
+        <v>-0.93390407406420295</v>
+      </c>
+      <c r="F45">
+        <v>0.64045501877975597</v>
+      </c>
+      <c r="G45">
+        <v>148.14637109925101</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0.68753464128658404</v>
+      </c>
+      <c r="K45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>21.943470000000001</v>
+      </c>
+      <c r="C46">
+        <v>48.94567</v>
+      </c>
+      <c r="D46">
+        <v>16.898598277863901</v>
+      </c>
+      <c r="E46">
+        <v>-0.69427318466002896</v>
+      </c>
+      <c r="F46">
+        <v>-1.8326814013197901</v>
+      </c>
+      <c r="G46">
+        <v>145.34700392278901</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>-1.9112025088415801</v>
+      </c>
+      <c r="K46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>21.94314</v>
+      </c>
+      <c r="C47">
+        <v>48.945320000000002</v>
+      </c>
+      <c r="D47">
+        <v>16.344513942230499</v>
+      </c>
+      <c r="E47">
+        <v>-0.47840213272946602</v>
+      </c>
+      <c r="F47">
+        <v>0.77393020010541003</v>
+      </c>
+      <c r="G47">
+        <v>144.35061495371801</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>0.79726609126511205</v>
+      </c>
+      <c r="K47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>21.942689999999999</v>
+      </c>
+      <c r="C48">
+        <v>48.944929999999999</v>
+      </c>
+      <c r="D48">
+        <v>12.725169861388</v>
+      </c>
+      <c r="E48">
+        <v>-0.37766097665134701</v>
+      </c>
+      <c r="F48">
+        <v>1.5551803370888899</v>
+      </c>
+      <c r="G48">
+        <v>143.854425963099</v>
+      </c>
+      <c r="H48">
+        <v>1</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>1.6027470916834099</v>
+      </c>
+      <c r="K48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>21.942209999999999</v>
+      </c>
+      <c r="C49">
+        <v>48.944569999999999</v>
+      </c>
+      <c r="D49">
+        <v>13.576707367445501</v>
+      </c>
+      <c r="E49">
+        <v>-0.71093150439750696</v>
+      </c>
+      <c r="F49">
+        <v>-2.2988035231839499</v>
+      </c>
+      <c r="G49">
+        <v>145.06442926716599</v>
+      </c>
+      <c r="H49">
+        <v>1</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>-2.4258298187177698</v>
+      </c>
+      <c r="K49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>21.941569999999999</v>
+      </c>
+      <c r="C50">
+        <v>48.944159999999997</v>
+      </c>
+      <c r="D50">
+        <v>10.8897535710054</v>
+      </c>
+      <c r="E50">
+        <v>-0.292444651200227</v>
+      </c>
+      <c r="F50">
+        <v>1.8686661737793799</v>
+      </c>
+      <c r="G50">
+        <v>141.13591775126</v>
+      </c>
+      <c r="H50">
+        <v>1</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>1.9202341172578601</v>
+      </c>
+      <c r="K50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>21.940829999999998</v>
+      </c>
+      <c r="C51">
+        <v>48.943739999999998</v>
+      </c>
+      <c r="D51">
+        <v>11.6946548072565</v>
+      </c>
+      <c r="E51">
+        <v>4.6849920453210597E-2</v>
+      </c>
+      <c r="F51">
+        <v>-1.7935285485478301</v>
+      </c>
+      <c r="G51">
+        <v>139.55641022383</v>
+      </c>
+      <c r="H51">
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <v>-1.7863721685285201</v>
+      </c>
+      <c r="K51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>21.94022</v>
+      </c>
+      <c r="C52">
+        <v>48.943440000000002</v>
+      </c>
+      <c r="D52">
+        <v>14.5675680103883</v>
+      </c>
+      <c r="E52">
+        <v>-5.4422221447791998E-2</v>
+      </c>
+      <c r="F52">
+        <v>-3.1452785682103501</v>
+      </c>
+      <c r="G52">
+        <v>149.16566866987699</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <v>-3.1570729130921098</v>
+      </c>
+      <c r="K52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>21.939609999999998</v>
+      </c>
+      <c r="C53">
+        <v>48.943190000000001</v>
+      </c>
+      <c r="D53">
+        <v>10.4758086885459</v>
+      </c>
+      <c r="E53">
+        <v>-5.3221144629195201E-2</v>
+      </c>
+      <c r="F53">
+        <v>1.9621886797897801</v>
+      </c>
+      <c r="G53">
+        <v>146.29919047031299</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>1.9722082576611</v>
+      </c>
+      <c r="K53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>21.938829999999999</v>
+      </c>
+      <c r="C54">
+        <v>48.942900000000002</v>
+      </c>
+      <c r="D54">
+        <v>11.385569558584599</v>
+      </c>
+      <c r="E54">
+        <v>-0.12106128210158</v>
+      </c>
+      <c r="F54">
+        <v>-1.59117021115827</v>
+      </c>
+      <c r="G54">
+        <v>149.53339602010701</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>-1.6082707450721001</v>
+      </c>
+      <c r="K54">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>